<commit_message>
separation of concerns axios
</commit_message>
<xml_diff>
--- a/Backend/media/planillas_excel/inventario.xlsx
+++ b/Backend/media/planillas_excel/inventario.xlsx
@@ -55,15 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -431,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,12 +436,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="17" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -482,62 +479,34 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>0111111111111111112</t>
+          <t>123456789</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Cigarrillos Camel x12</t>
+          <t>caraca</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>978.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>2500.0</t>
+          <t>200.0</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>2022.0</t>
+          <t>100.0</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>TiendaClick</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>lol</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>1000.0</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>100.0</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr"/>
+          <t>Sin proveedor</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>